<commit_message>
Get daily reddit data: Tue Jun 10 08:13:10 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_15.xlsx
+++ b/data/collected_data/2025_06_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C494"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3287 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1l7sy3q</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>my sister did my nails for my chemistry exams</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7sy3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1l7sx5j</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Oval or square?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7sx5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1l7scds</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Finally mastered isolated chrome</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7scds</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1l7s4ji</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>A subtle '❤️💜💙' moment.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7s4ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1l7rt7s</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>tb to the longest my nails have ever grown to &lt;/3 im trying to grow them out again</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7rt7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1l7qwk9</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>What’s ‘up’ with my nail?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6d9yk4xd16f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1l7pdab</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>I did these nails for my boyfriend, but I think I still need to improve. What do you think?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mbuexinx06f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1l7qasd</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Had to share the best set I've ever had done.</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aq9v5818716f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1l7pnx4</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>What Nail Shape Is This?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tpb7tgk016f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1l7ptpe</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>a manicure especially for summer</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mis1gg74216f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1l7p14q</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Weeks old, but cute.</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7p14q</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1l7oknf</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>My new nails (gel done by me)</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f9srs3wp06f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1l7ogu2</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>7 weeks of growth on my natural nails to new manicure:)</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ogu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1l7ob5c</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>My Newest Gel X Set!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75rmocaen06f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1l7n9gm</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Red orange, anyone?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cy6hngptd06f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1l7o5dp</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>blue and pink for my 5th gelx set</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7o5dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1l7nlyl</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Fresh manicure today :)</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvvya96xg06f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1l7nkdh</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Living my cutesy dreams</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7nkdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1l7njty</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Almond or squoval?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7njty</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1l7nfpy</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Pride Nails!!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7nfpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1l7lbpr</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>New beach set</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7lbpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1l7mmpi</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Witchy woman</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzuboda5806f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1l7mewb</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>I have to break up with my nail tech 🥹</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l7mewb/i_have_to_break_up_with_my_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1l7mcd5</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Cute Blue Press ons 🩵</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7mcd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1l7m487</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Pearly whites</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7m487</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1l7lzpt</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Every time I paint my own nails with gel polish it peels off almost instantly??</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l7lzpt/every_time_i_paint_my_own_nails_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1l7ltrb</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Convocation nails</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ltrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1l7lk4z</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Nail designs to go with this dress</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzpw2qnqyz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1l7l5sg</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>so cute and summery :))</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7l5sg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1l7l51f</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Fun design today 💘🦋🔮💐🌸</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mp4o2kb2vz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1l7kp3y</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>My amazing nail tech made me so happy yet again 🌸🍓</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9m1smfl8rz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1l7khdm</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Any nail techs ever find their own work in these comments and/or posts?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l7khdm/any_nail_techs_ever_find_their_own_work_in_these/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1l7kar4</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Best Gel nail builder to buy from Amazon!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l7kar4/best_gel_nail_builder_to_buy_from_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1l7k5ng</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>First magnetic mani 😍</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tfjquwlsmz5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1l7k12d</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>June is my favorite month to do nails, I think :)</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7k12d</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1l7jg1c</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Doing my own nails</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7jg1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1l7je7o</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Before the magic happened.</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7je7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1l7ivop</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>I've not bitten my nails for over a year now!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ivop</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1l7j7bv</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Gimme nails like a summer sunset✅</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sib5xcm3fz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1l7j2id</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>These feel like accidental renaissance</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7j2id</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1l7ith5</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>are these bad??</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ith5</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1l7is5y</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Pride Nails!</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwz8zkhrbz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1l7inru</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Did my nails in celebration of getting my license 🥰</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7inru</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1l7ij0p</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>What can I do to strengthen my nails?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j4dxg9os9z5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1l7hy4v</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Simple cutesy fresh set 💕</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7hy4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1l7geyh</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Beginner Help with Gel</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l7geyh/beginner_help_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1l7hapr</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>The difference nail shape makes</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7hapr</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1l7h24n</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>summer nails!🩷💜🤍</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggoe1dlyyy5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1l7gzmm</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Should I remove these?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7gzmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1l7ga3y</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Crying cause of the nail tech</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22bsns1gty5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1l7gtu6</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>New set ✨🌺</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7gtu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1l7gm47</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Cyber Milk press on set 🖤</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1kz5u51pvy5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1l7gldn</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Gel- X hand painted chrome and glitter butterfliesss - it’s giving y2k hehe</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdufixsmvy5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1l7g9hu</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>The Nails Bae Pink on Pink French Gold Trim GEL-X. What you guys think ?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kjpcujbty5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1l7fpvf</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Hema Gel Nail Polish VS. Hema-Free</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l7fpvf/hema_gel_nail_polish_vs_hemafree/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1l7g07z</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Remove TAP for Korean press-on?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l7g07z/remove_tap_for_korean_presson/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1l7g250</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Is this normal after a week?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7g250</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1l7fpjf</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Gel manicure lifting after 4 days?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7fpjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1l7fiui</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>I have a funeral tomorrow; I painted my nails for it ☺️</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4krsovj6oy5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1l7enu5</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Gel polish cracking</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/joexye0diy5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1l7f7g8</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I did this work today, do you like it?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efw4rt91my5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1l7f4db</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Builder gel fill!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7f4db</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1l7f3yz</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Literally the perfect nude</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7f3yz</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1l7eeb7</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>vacay nails!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lirnp1kgy5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1l7e8sx</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>A guy I like once told me he thought short, delicate nails looked more elegant.</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7e8sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1l7btta</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>These are everything.</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/92qqgmguyx5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1l7bvt7</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Monet Cats</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7bvt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1l7e1fb</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>First GelX application, any advice?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7e1fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1l7dx1r</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Dip Powder Help!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ouyavn9dy5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1l7dkec</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>2nd acrylic gel set, any tips or advice appreciated!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7dkec</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1l7dh3v</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Holiday nails. Never posted on here as I have horrible nails and hands but I loved my recent spring holiday manicure with lemon tips.</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tctibpp8ay5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1l7d4w4</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Made by me :)</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0js2pa6y7y5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1l7cxil</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Mermaid nails</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7cxil</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1l7cwdg</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>First time nails — worried about the angle?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7cwdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1l7ct4h</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Painting help!</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ct4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1l7cpbn</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Yay or nay? I'm loving them</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi456jhy4y5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1l7bjgj</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Any notes?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7bjgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1l7cet5</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>A fun girly set I did back in early March</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7cet5</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1l7c4d3</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>I'm in love 🥰</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7c4d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1l7c2zm</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Soft touch flex</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urm5tcnm0y5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1l7by1f</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>My gorgeous textured birthday nails</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7by1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1l7bx28</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Just nails</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7w7zxqhzx5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1l7bv6w</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Needed A Pick-Me-Up</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpydksb4zx5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1l7bq4e</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I’ve spent the last 29 years biting my nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cre5krx5yx5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1l7bn4u</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Never thought I'd be the girl to look at my nails 50 times a day 🥰</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3ltt00mxx5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1l7blbr</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8f8juw8xx5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1l7b0y0</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Usually a neutrals girl but tried “Pink Chrome” :)</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rfn3kxgtx5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1l7angz</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Help with impress bubbles</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7angz</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1l7am1b</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Glitter and Gold</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7am1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1l7ac89</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Pokémon Emerald inspired emerald green! 💎🟢</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ac89</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1l79wx6</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Feedback?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l79wx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1l79bup</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Allergy to ORLY BIAB?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l79bup</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1l79rhq</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Bloood orange slices 🍊</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odi8c7qukx5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1l79ggp</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>I love my new set</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l79ggp/i_love_my_new_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1l7410u</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Salon rant</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7410u</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1l78z6w</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>summer mermaid 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l78z6w/summer_mermaid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1l78m1l</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>My one year progress</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l78m1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1l78gen</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>fresh nails!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yq4tk6isbx5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1l77tye</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l77tye</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1l77ri4</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Summer nails 🍒🌸</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jqc33rx6x5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1l7t5ym</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Think I found the perfect nude</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4tb9sfl326f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1l7s091</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>How to avoid the toad effect</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aemqyhmuq16f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1l7r4wb</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>I feel like a crazy person for saving all my packaging, but moving is way less stressful now.</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7r4wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1l7qyft</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>PPU Dupe Requests and Immediate FOMO</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7qyft</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1l7pv1p</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Bees knees lacquer</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l7pv1p/bees_knees_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1l7prb2</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Emily De Molly sheer tints?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l7prb2/emily_de_molly_sheer_tints/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1l7pqia</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Your favorite (available) neon green?</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l7pqia/your_favorite_available_neon_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1l7p7iw</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Messy nail art 😅</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7p7iw</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1l7ndlv</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>My attempt to recreate pixel perfect gradient by u/Shoogalooga</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vr7ngoif1z5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1l7mxey</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>First time buying ILNP</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7mxey</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1l7mrnw</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>I’m in love!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tye8li3e906f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1l7mnjl</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Do you find yourself wearing a color at specific times?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7mnjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1l7melf</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>experiment…..successful?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t374lyg4606f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1l7l3m5</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Maybe been scrolling too long  . . .</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93r19akgtz5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1l7l1x9</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Fancy gloss shipping time?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfqu1i1buz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1l7kyka</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Finally, after eyeing this shade for years… ILNP - Amber</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eqcxb2xgqz5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1l7kuyw</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>jelly sandwich! Collecting seashells</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snm83zfmsz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1l7kh8p</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Cracked - Pistachio Buttah + DVN</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4flk20ifpz5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1l7k0pf</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>A little blue for the summer heat</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7k0pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1l7jv9v</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Joining the hypnosis hype.</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bwkkk7vfkz5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1l7ji32</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>There is really no way to capture how insanely shifty this one is!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u97twp0chz5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1l7j9qa</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Hypnosis - ILNP omfg</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7j9qa</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1l7ixrx</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>OPI Without A Pout</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ixrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1l7ish5</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Magnetic troubleshooting</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ish5</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1l7iog5</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>I absolutely love how many colors Forbidden Fruit offers</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0bmd72oyaz5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1l7iade</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Zoya Alma — happy yellow sparkle!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/07x691yy7z5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1l7hsvg</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>{PR} 🌺 Just Got Lei’d by @sassysaucepolish 💅 🍹</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7hsvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1l7hnex</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>What is the standard price for a thermal?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l7hnex/what_is_the_standard_price_for_a_thermal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1l7h6vf</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>A little swatch game?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7h6vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1l7fme2</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Mexican Talavera Terracotta inspired mani!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wdhom5ioy5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1l7fuvf</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Summer Blue 💙💙</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7fuvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1l7g5bo</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Grotto 💙</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7g5bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1l7fc1b</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Watch me awkwardly wiggle my fingers</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0lgtr58umy5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1l7ewiu</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Mega (X) for the Rainbow Vibes</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ewiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1l7dm9b</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Dreamy is so dreamy</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7dm9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1l7cros</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Purple Moon💜🤍🌙</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7cros</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1l7cq0f</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Looking for a aubergine jelly nail polish</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l7cq0f/looking_for_a_aubergine_jelly_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1l7ckhl</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Magnetic polish is my new obsession</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/us4osiv04y5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1l7c1c5</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>What am I doing wrong for my cuticles to be so —- flat?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldumdrhb0y5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1l7bp0m</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Flakiessss</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7bp0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1l7blku</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>BKL Shadow Daddy and Arcane</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/09li6gyaxx5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1l7avsf</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>My Life as a Mollusk 🦪</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7avsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1l7ajf5</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈🩵💛Pansexuality Pride Flag💛🩷🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7ajf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1l7abch</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Dupe for MC hardcore base?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l7abch/dupe_for_mc_hardcore_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1l7aad7</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Retrowave Manicure</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxcct0r8ox5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1l7a4yi</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Gradients all day everyday!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7a4yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1l79jiy</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>A little bubble space and kitty mani</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l79jiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1l79ev3</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Glow-in-the-dark rainbow mani in action</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wxku01j1ix5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1l78skz</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Had to show off</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6jk26h2ex5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1l78o4b</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>polish chipping from only tips</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2frq5u8dx5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1l78nmo</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Palace 💅</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l78nmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1l780iu</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Norpsilocin velvetized 🤩</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l780iu</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1l77qa9</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Happy Pride! ❤️💜💙</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nvbplbpk6x5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1l77q0f</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Mini haul brag! My little adhd brain and black heart are satisfied now (for a while at least)!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sfntofeq5x5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1l77j30</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>ILNP Sugar Plum vs Cirque Kinetic? Or any rose-y mauve magnetic or jelly to top?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l77j30</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1l77faw</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Anyone BTS fans here? Looking for the perfect purple color match for their iconic purple, picture included!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l77faw</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1l773lv</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Mooncat Millennia 🤩</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yb1mw4e52x5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1l76qzs</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Dupes for Mooncat’s “Treachery in the Blue”? I’m not paying $18 for a thermal 💀</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soyczooszw5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1l76oo9</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Porcelain nailart</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l76oo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1l76fcc</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Loving this color ❤️</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l76fcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1l76bo0</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Flower Bridge</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l76bo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1l760ee</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Just discovered magnetics</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l760ee</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1l75bqp</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Loving my new lavender milk nails!</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scb6jypepw5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1l759fo</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>color i ♡ &amp; musings of the struggle to get an accurate pic of it</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l759fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1l74o6b</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Dupe for Beauty Pie Super Nude?</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l74o6b/dupe_for_beauty_pie_super_nude/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1l74923</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>My nails are literally GLOWING and I can NOT handle it!</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pc3wjnrwgw5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1l74875</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>6 day manicure 💅</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l74875</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1l72opn</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>So nice to see progress :) Nail Glow Up</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l72opn</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1l72ccj</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat Fallen Angels?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l72ccj</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1l71j9g</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>How to care for nails properly?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5t1oqpzrv5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1l70v90</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l70v90/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1l6zjxe</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Magnetize just hits different sometimes</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e59depwx4v5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1l7qfmp</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Summer beach nails! 🌊💙</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7qfmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1l7qfki</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>My very first attempt at doing my own nails at home</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7qfki</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1l7pv5n</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>All the nails I did last week + the last! (Open to suggestions of what to do next!)</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7pv5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1l7otgu</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>First time making a Harry Potter deco, the photo was different, I put my drawing style on it 🥹... do you like it? I was shocked at what I could do 😭😭</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7otgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1l7odwy</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>She want classy with a kick. How I do ?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d36be234o06f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1l7oa97</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>my first attempt at sculpting gel!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9tp2xt5n06f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1l7nh8f</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Nails for Pride!!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7nh8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1l7moxz</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Nail designs to go with this dress</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l7moxz/nail_designs_to_go_with_this_dress/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1l7l7a8</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Finally used the Ghibli stickers in my collection ✨</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzj6nsblvz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1l7l232</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>My semi sad attempt at beach nails.</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxcwx7lcuz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1l7kvl0</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Nails ive done&lt;3</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7kvl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1l7k9qq</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>I cannot seem to get nail stamping polish to show up! It's so sheer, patchy, and difficult to do!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7k9qq</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1l7geus</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Cyber Milk press on set 🖤</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p1n62o8auy5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1l7fnqi</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Where to get press ons?</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l7fnqi/where_to_get_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1l7f5l3</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Tried to recreate this look i saw on Instagram (nail tech info on second photo)</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7f5l3</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1l7e749</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>nail set help</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ii6q82u6fy5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1l7c7iq</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>A fun girly set I did back in early March</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7c7iq</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1l7b44u</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Summer nails done by me! 🥥🐚</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7b44u</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1l73ebh</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Did My Sister nails last night, how did I do?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l73ebh</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1l7269g</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Cateye &amp; Pearls</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdfz6a3gyv5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1l71t4r</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Plain vinyl sticker sheet</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l71t4r/plain_vinyl_sticker_sheet/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jun 11 08:12:57 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_15.xlsx
+++ b/data/collected_data/2025_06_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C494"/>
+  <dimension ref="A1:C685"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8831,6 +8831,3253 @@
         </is>
       </c>
     </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1l8mpwb</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Did my niece's nails for her graduation☺️✨</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8mpwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1l8mjr9</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>First time getting my nails done!!</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8mjr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1l8ks57</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Started doing my own nails and I’m loving it!</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8ks57</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1l8jlxe</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Almost 4wk old Luminary &amp; DND gel salon nails and I can make an impression of my nail into the gel…is this normal?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8jlxe/almost_4wk_old_luminary_dnd_gel_salon_nails_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1l8kzt8</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Still a beginner but newest set!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qz29jx6jl86f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1l8kpcr</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>capping gel</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wz898i5i86f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1l8jqn0</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Need help with pedicure!!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8jqn0/need_help_with_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1l8irqe</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>upset</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8irqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1l8jbfw</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Blueberry 🫐</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p18ouuih386f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1l8j9r6</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Did my own nails today (my natural nails)</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1a8w3hz286f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1l8j541</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Absolutely loving this set</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0whi9ju186f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1l8j096</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Long nails with ribbon</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8j096</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1l8is1d</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Velvet meow nails 😻</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/udvx9ph7y76f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1l8io8f</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Simple 🤍🩷</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8io8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1l8i0zz</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Love this color ❤️</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4j7crem0r76f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1l8hxa3</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>So in love with my nails</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/px3vn5h2q76f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1l8ht9v</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>my first time using Luminary + gel polish</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8ht9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1l8hlzr</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Alice and Wonderland vibe nails!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8hlzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1l8hlcx</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Happy Pride🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8hlcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1l8h6qr</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>How’d I do??</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8h6qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1l8h5jr</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>nails for Disney/birthday 🌟🥰🩷</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/og2mv2d2j76f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1l8h0hs</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>✨ &amp; ♥️</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/308qsjsth76f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1l8gue4</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Favorite set of the day✨</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/unwx9c4cg76f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1l8gm52</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Straykids nails art</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8gm52</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1l8gart</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>I love doing my own nails!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8gart</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1l8g3hc</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>What shape should I go for?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2kyvwyh976f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1l8fwsx</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Shakey Hyperthyroid hands! Halp!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxcyofrt776f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1l8fmhu</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>We painted each other's nails!</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4luyrw68576f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1l8fdwp</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Pride 2025 🏳️‍🌈🌈💅</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8fdwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1l8fgff</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Happy pride !!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8fgff</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1l8fesl</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Is a foot pedal for a nail drill worth it?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8fesl/is_a_foot_pedal_for_a_nail_drill_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1l8ewr2</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Monet inspired set</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8ewr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1l8f5j8</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>asked for gel building, tech did hard gel instead</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8f5j8/asked_for_gel_building_tech_did_hard_gel_instead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1l8ewjh</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Growing and painting them myself. A work in progress for my self control</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqsmfyxwy66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1l8eueq</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Clean and smoooov</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpz393lgy66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1l8emzo</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>New Set (ready for Electric Forest)</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8emzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1l8eekg</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Short nail beds, I have no idea what I’m doing</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8eekg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1l8ecyk</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Advice to improve</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8ecyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1l8e2ys</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Walked past a matching rose</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6kqff40s66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1l8e1tf</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Classic nails.</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcutsxgqr66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1l8dxd6</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Gel polish</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tst334qq66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1l8duy4</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>First time doing my own gel nails!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wn7qqn4q66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1l8dtfu</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>BIAB Nail growth progress photo</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylp1001up66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1l8ds7x</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>First time with Rojo ❤️</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq3s76bkp66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1l8dnev</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Mom and daughter nails</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhtpj3lgo66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1l8dka9</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>would you get a fill yet?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjvb242rn66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1l8dgnk</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Gel X nail was only put under UV for a short time</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8dgnk/gel_x_nail_was_only_put_under_uv_for_a_short_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1l8cyql</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Nail Polish Question</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8cyql/nail_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1l8d2nd</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Early 2000s pattern nails I did on myself</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8d2nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1l8cjqv</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Happy pride! 😊 🌈 💅🏻</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqzv8iavf66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1l8cafz</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>First time getting acrylic nails done</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8cafz</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1l8c4ou</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>poison ivy x harley quinn nails for pride month!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au4bftwlc66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1l8c038</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>damaged nails?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie6bjgymb66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1l8c169</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Creating a coraline nails set with some special effects</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/97sfvv5vb66f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1l8bpj5</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Behold – my latest set!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3zl75sg966f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1l8bocx</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>chinese nails for aapi month</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24xpc7e8966f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1l8bdfz</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Birthday Set</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/916qbapz666f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1l8b7yv</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Not what I asked for</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2yripyv566f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1l8b4t9</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Happy Pride!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttegqcq5566f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1l8b0hx</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>New set after months of bare nail, feeling good</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8b0hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1l8azpz</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>🌌 ❤️</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8azpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1l8aq8r</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Nail Tech Refused To Do My Nails After Removing Gel Polish</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk1e9dxa266f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1l8ap3a</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>First time doing my own acrylic nails in a long time, please don't be to harsh. Don't mind the polish on side of fingers ran out of polish remover.</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8ap3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1l8an7d</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>New manicure! Happy Pride! 🌈</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mlz7iap166f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1l89z65</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Do you like glitter on your nails?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nujvvdn1x56f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1l89h58</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>What would you do?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l89h58/what_would_you_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1l890b1</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Any Alternatives?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l890b1/any_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1l897dp</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>New summer mani 🤍</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uorbkmolr56f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1l893k3</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I went to get my nails done and they came out like this… I’m so upset</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijc20osvq56f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1l88yp1</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Thinking of growing my natural nails out after this set, any tips?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olmym26zp56f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1l88twg</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>My first summer set! 🥥🐚</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l88twg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1l862b1</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Nail tech did not adhere to inspiration photo</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l862b1/nail_tech_did_not_adhere_to_inspiration_photo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1l88l38</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>FINALLY...no peeling on the tips!</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp2fl1mdn56f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1l86q4y</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Romantic denim set</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l86q4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1l884q2</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>my nail artist doesn’t know how to stop slaying</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l884q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1l870d4</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Can you put a gel top coat over nails strips to seal them better?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l870d4/can_you_put_a_gel_top_coat_over_nails_strips_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1l86jdn</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>My press ons from Amazon 💕💕</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l86jdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1l85203</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>What shape works best for me</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l85203</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1l83lte</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Chrome nail powder without gel</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l83lte/chrome_nail_powder_without_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1l84xbj</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Nail Diy</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43bet81ay46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1l84v6d</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Is there any way to grow paper thin nails longer and thicker?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l84v6d/is_there_any_way_to_grow_paper_thin_nails_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1l84ut1</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Pink and yellow ombre 🧡💛🩷</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g917i3zsx46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1l84ly6</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Early attempt at shellac nails</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l84ly6</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1l84bhl</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>I just got my nails done!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akh6vkvvt46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1l849by</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>What nail shape should I ask for?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l849by</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1l848i3</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Good or Bad?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l848i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1l844is</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>I was going for something really sparkly this time ✨</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l844is</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1l840ef</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Summertime</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l840ef</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1l83xj5</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Just finished them last night</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0twxzzwkr46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1l83x5t</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Feeling sweet and girly with my new nail art and nail length even as a guy</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l83x5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1l83dgi</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>French Tip Base Color</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l83dgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1l82ykf</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Outside my comfort zone</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3knznjrk46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1l82uwc</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>My gel polish keeps peeling off after just a week</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l82uwc/my_gel_polish_keeps_peeling_off_after_just_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1l82tfj</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>New mani, who dis</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l82tfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1l82ov1</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>My new nail set</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mrbzptti46f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1l82dy8</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Summer Vacation Nails 👸🧡</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l82dy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1l824c3</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Pretty or not?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l824c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1l81gi7</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Finished my honeymoon nails!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l81gi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1l81dh9</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jvjklrn946f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1l8149a</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>First time trying 3D nail art and obsessed is an understatement. My nail tech always kills it!!</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8149a</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1l8l2o2</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Polish won’t dry with Seche Vite?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8l2o2/polish_wont_dry_with_seche_vite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1l8kfkn</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Large press-ons for wudu rings</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8kfkn/large_pressons_for_wudu_rings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1l8k7a6</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Completed Collection...?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqxzfppjc86f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1l8ju3h</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Inspired by nail stickers: Mooncat Apollo w/ holo nail stickers &amp; chrome powder</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7zxmxw0r886f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1l8jqsw</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Forgot how much I love white nails 🦷 Essie TLC - In A Blush</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8jqsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1l8jjao</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>First try with gel</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8jjao</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1l8ifr1</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Yet Another Rainbow!</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ij4z3kdxu76f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1l8hzgr</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Indies Like This?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8hzgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1l8hl6g</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Trans pride mani didn't really turn out how I envisioned, but still lovely</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sambq6e0n76f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1l8hdit</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Can ya’ll recommend a pink and milky, light blue very very similar to these?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8hdit</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1l8gjb7</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>first cirque purchase!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8gjb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1l8geo3</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Building a timeless nail polish collection - missing anything?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jq24krbc76f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1l8gdw8</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Mooncat nail file question</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8gdw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1l8g4ev</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Another one bites the dust... is it weird to have one hand short, one long or can you make it work?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hks9m63q976f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1l8fcfb</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8fcfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1l8f1oz</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Glisten and Glow Lets make a splash vs Lurid Joie de vivre vs Lurid diaphanous dreams swatches for comparison?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8f1oz/glisten_and_glow_lets_make_a_splash_vs_lurid_joie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1l8evtt</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Couldn't decide on a polish so  I did something different on each hand</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8evtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1l8emyk</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>really didn’t wanna like this one</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8emyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1l8ehlc</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>I'd have a question about quick dry top coats-</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8ehlc/id_have_a_question_about_quick_dry_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1l8dozd</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>A beautiful shade that I hate for some reason? Tried by itself and over various cremes.</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8dozd</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1l8do44</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Glass nails, various magnetics under Starrily Jelly</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u3mr7rzjo66f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1l8djcn</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Broken HHC Polish</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kc4h3zin66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1l8cy3i</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Can finally contribute to the ‘duped myself’ discourse</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8cy3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1l8car7</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>The little things matter ILNP</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8car7</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1l8bsly</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>has anyone done these with magnetic lacquer instead of gel?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8bsly</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1l8brtd</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Matching Nude Polish with Skin Tone</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8brtd/matching_nude_polish_with_skin_tone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1l8bm0e</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Watermelon 🍉</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8bm0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1l8bfv5</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>pride mani #2: juicy rainbow!</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8bfv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1l8armg</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>May's Manis</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2j4i8kl266f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1l8aret</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Blue(berry)lagoon</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l820xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1l8ar0y</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>They're heeeeeere!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8ar0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1l8aidr</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Dystopian Daydreams</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf653fyr066f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1l8af5v</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Cracked Polish Shipping?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8af5v/cracked_polish_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1l8aav5</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Flakie Texture</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6my789bz56f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1l8a0zv</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Polish that stays</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8a0zv/polish_that_stays/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1l89kqj</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Shiny rainbow for Pride!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l89kqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1l8854r</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Recs for this bright purple?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oicll559k56f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1l883wj</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Your orchid tariffs are killing me</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l883wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1l883dm</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>The Perfect Red</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l883dm</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1l87rlk</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Blue Cross cuticle remover made my nails hurt almost immediately, OW!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l87rlk/blue_cross_cuticle_remover_made_my_nails_hurt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1l879kq</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>What color is this?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlz18j25e56f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1l85p0h</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>👻💩</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l85p0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1l854nx</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Purple multichrome for BTS reunion week!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l854nx</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1l84olr</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Just did these :,)</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l84olr</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1l84dr5</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>I love this bold blue color but…</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l84dr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1l846h8</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Paint job help</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ied9wdk7t46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1l83z1l</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Haven't quite mastered chrome powder on normal polish yet, but I'm still obsessed</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l83z1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1l83gpz</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Ugliest mani ever</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oepcu5rbo46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1l83cz2</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Oddities🍏</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l83cz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1l82r3u</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Mooncat - Tectonic Shift</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l82r3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1l82kx0</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Beaux Reves Customer Service 10/10</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l82kx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1l82erm</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Glowy skittle!</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qoeyxtxg46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1l82e9c</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>June Rainbows 🌈</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l82e9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1l81hgh</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Glowy blurple</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7ijt8nfa46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1l80tzg</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Swatch question</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l80tzg/swatch_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1l80mi6</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Wanted to share my pride nails, too 🩷💛💙</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l80mi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1l80l4l</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>First time trying out gradients ✨️</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gm21rz76446f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1l80h07</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Holo Taco Bonus Life</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l80h07</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1l800jf</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>What brands to try?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l800jf/what_brands_to_try/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1l7zitu</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Essie to the rescue: a love story?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yckvanoew36f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1l7yqof</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Testing a glitter suspension base as a smoother</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ib8ypz8dq36f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1l7yqvn</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>🏳️‍⚧️🏳️‍⚧️🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7yqvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1l7yawh</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Holo Taco Shimmering Secrets ✨🔎🩵</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7yawh</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1l7y7cw</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>does anyone in this subreddit else use instagram to document their manicures?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujna6wh2m36f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1l7oqkl</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Help- What type of gel should I use to make my grandma’s nails durable and pretty?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l7oqkl/help_what_type_of_gel_should_i_use_to_make_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1l7xcd1</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Round 2 of Glass Nails: bubbly and messy, but - a successful attempt!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7xcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1l7x6m5</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Emily de Molly autumn skittle</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7x6m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1l7x23h</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>I did these in bad lighting last night, now I'm not sure. What do we think?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25tb9jq7c36f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1l7wrbg</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Are those air bubbles?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7wrbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1l7uu5u</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l7uu5u/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1l7upmh</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>My finger slipped 😬</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jziruqi3o26f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1l7uhdh</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Love wins 🌙 🌈 ⭐</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7uhdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1l8m6n8</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Black and White Nails done by me</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dfwsicjz86f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1l8gfwe</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Summer is too hot. Can I go back to spring? 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siz572dnc76f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1l8hta2</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>A close up of my koi fish set</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pqdt6oizo76f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1l8fa2z</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Pride 2025 🏳️‍🌈🌈💅</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8fa2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1l8ctzj</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>First time posting to Reddit</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04de0bq1i66f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1l8c09v</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Playing about with heat activated powders with this scene from coraline 🥰</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/upb3xb5ob66f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1l8btzp</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>my nail bestie did Harry Potter nails for me</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8btzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1l7kdfi</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Who said u can’t have design on short nails? 😚</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uxwapekoz5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1l7rq8r</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>in need of critiques</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l7rq8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1l884ir</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>my melody nails</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l884ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1l87tn1</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Looking for beginner advice</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l87tn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1l86rd6</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Romantic denim set</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l86rd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1l84evy</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>spring nails 🌷</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kjc56mtu46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1l83noe</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>for the shell of it! 🐚✨</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l83noe</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1l834vq</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Square nail set done by me</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g857duphl46f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1l82z42</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Something more subtle for my trip</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00el8uhvk46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1l81ktp</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>🧜‍♀️ Nails</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ls5fgu03b46f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1l800y6</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>delicate pink 🩷</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xrqrmu3046f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1l7v6t0</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>✨️💓</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7byay8ft26f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jun 12 08:13:04 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_15.xlsx
+++ b/data/collected_data/2025_06_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C685"/>
+  <dimension ref="A1:C877"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12078,6 +12078,3270 @@
         </is>
       </c>
     </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1l9gmac</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>What do you all think?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wn6o95gbg6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1l9g06q</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9g06q</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1l9g016</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Too short?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txbcmmzy3g6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1l9fa0x</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Hello summer 🍋</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9fa0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1l9ezww</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Simple cat eye</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3emi2nhbsf6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1l9etwf</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>First time getting my nails done and I already want to take them off :-(</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc9a6erfqf6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1l9exmk</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Practicing a snakeskin chrome nail for a press on set. What do we think?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zx2y4d4jrf6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1l9ehg1</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>First attempt at a french manicure!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9ehg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1l9dztc</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Summer nails!</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8755dk3hhf6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1l9dczl</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>My homemade press-ons💜✨</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/je78qgzvaf6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1l9d4b3</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>New homemade press-ons💜✨</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9d4b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1l9cvwj</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>PRIDE</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svy7jw766f6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1l9cd53</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Pride nails!</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9cd53</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1l9c287</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Love this colour 🥰</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9c287</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1l9c0u6</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Color Suggestion?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djylexluxe6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1l9brg5</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>my favorite full set</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9brg5</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1l9bmk6</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>I love my nail artist!</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tosb0093ue6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1l9bicm</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Doodlebob</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w18o580te6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1l9bflm</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Strawberries!!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ne0sex8ase6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1l9ak1f</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>plsss change my mind about my nails</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9ak1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1l9apfk</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Mooncat - Twilight Sonata</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9apfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1l9b7hj</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>At what point do you just get up out of the chair? i was vocal and outspoken throughout the entire process but wasn’t enough…</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9b7hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1l9baru</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Please help me! How can I get nice long feminine nail beds?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9baru</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1l9a5gg</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Bendy nails with ridges</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9a5gg/bendy_nails_with_ridges/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1l9a1as</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>first time removing nails at home..</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9a1as</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1l998gz</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Nail Tech Seemed Overwhelmed by Pride Nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l998gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1l99i1p</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Advice?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l99i1p/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1l99faw</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>New to false nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l99faw/new_to_false_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1l99bkn</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Please, recommend a nude color for my nails?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypjmx9nm9e6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1l99b5t</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Hand painted nails for tonight's Halsey concert</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l99b5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1l992fz</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Gel pooling</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l992fz</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1l96t1g</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Faded Rainbows</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l96t1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1l97fud</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Vertical indents and ridges?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l97fud/vertical_indents_and_ridges/</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1l98djs</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Black shellac V-tips</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l98djs</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1l97jgk</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Ring of Fire?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l97jgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1l97d21</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i3wjo3ysd6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1l971os</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>I always get black or French - huge branch out day 😭  idk how to feel .</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yw1zd0vcqd6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1l97158</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>What are your favorite non-glue press-ons brands that DON'T get stuck in your hair?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l97158/what_are_your_favorite_nonglue_pressons_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1l96x7v</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Ombrè Stars for Pride!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l96x7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1l96unm</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>I loved it</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi3o71vsod6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1l96op8</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>French tip 💅</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rscsm5hnd6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1l95m4l</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Tried this new pearlescent shade my nail stylist has, thoughts?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brel0r8bfd6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1l95lvr</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Happy Pride 🏳️‍🌈🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l95lvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1l95ll5</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Matched my nails to my Subaru!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l95ll5</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1l90zo5</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Wedding nails… opinions?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pqs06f5ic6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1l953c6</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Opinions on nail shape?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yoh2izhbd6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1l9538x</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>DIY Summer Lemon Set</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdcu81ehbd6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1l948pc</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Is it air? Is it normal?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydkwmlmd5d6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1l951ky</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Feels good to be back 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24zdtl45bd6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1l93xdi</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Do it by myself</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l93xdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1l93oaa</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>June nails 🦋🌀🩵🫐🐬 (done by Jocelyn @ Get Nailed)</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45dong881d6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1l93ly7</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Nail success</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l93ly7</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1l93hzn</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Fruity fresh set for the season🍒</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l93hzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1l93fpm</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Can you put a gel top coat over regular nail polish to make them last longer?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l93fpm/can_you_put_a_gel_top_coat_over_regular_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1l915i9</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>How do you grow out your nails white? I have kind of transparent/translucent type of nails.</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l915i9/how_do_you_grow_out_your_nails_white_i_have_kind/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1l93dbk</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Views on straight men painting nails?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjp6inyyyc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1l93clv</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Obsessed.</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llb3afltyc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1l92aiu</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Inspired by princess peach 👑</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l92aiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1l91dec</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Sticky tabs or glue for a few hours</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l91dec/sticky_tabs_or_glue_for_a_few_hours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1l92yt3</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>my fish nails :)</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yg655sh1wc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1l92u72</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Tried a "thick glitter" on my toes. I like the glow, not so sure about the texture.</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dbvfdp4vc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1l92m14</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Pretty Blue 🩵</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l92m14</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1l91oug</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Time for a fill or go 4 weeks?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udh7pdg0nc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1l91orb</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>my pride claws</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l91orb</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1l91oiy</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Nail tech damaged my natural nails when removing gel polish</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l91oiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1l91d06</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Cinnamoroll nails!</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s1i3bfpkc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1l91cnn</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Lovey Dovey Clowns</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l91cnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1l91bvb</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6575gb6hkc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1l91a2q</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Subtle Rainbow Pride flowers</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l91a2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1l917g4</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>DND gloss moon 💜</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1h8hiujkjc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1l90hew</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Siren nails🧜‍♀️💙</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jj3tugjjec6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1l90825</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Nail designs and Acrylic</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l90825</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1l9079k</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>First BIAB and after 2 and a half weeks, 3 nails peeled off. Is this a normal amount of time for them to last?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9079k</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1l905gm</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Red Chrome ❤️</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c444k3u8cc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1l903qw</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Gift for my Tech</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l903qw/gift_for_my_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1l8ztka</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Femme mode is fun</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8qqgr9x9c6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1l8zjxd</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>can i go to a nail salon and ask them to paint the under side of my nails as well as the tops of them?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8zjxd/can_i_go_to_a_nail_salon_and_ask_them_to_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1l8zbxh</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>My long male nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9sunbbg5c6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1l8z978</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Can I mix dip powders?</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8z978/can_i_mix_dip_powders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1l8yzax</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hb1c28w64c6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1l8yn9r</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>New nails for the weekend 💙</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eepmmigu1c6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1l8ydsz</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8ydsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1l8y8j1</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>🌸</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/coqukbu1zb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1l8y08u</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>June press ons</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7p5ef56ixb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1l8xuy1</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Crooked fingers but make the nails cute 😂 ❤️</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7s45j4jwb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1l8xsdf</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>What can I do to fix them?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8xsdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1l8xp3y</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Thoughts? &amp; how much would u pay for it</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/caj4gjhdvb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1l8x9jo</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>ILNP - Flower Child</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8x9jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1l8x69w</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>i usually dont like red on myself but i had a dream about this</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gi3lvb8grb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1l8x38c</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Very happy with these beauties today❤️</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y9fqnwzqb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1l8x2l3</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Color!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffj2g9ovqb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1l8wt2s</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Lavender chrome nails 💅</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0emdz40pb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1l8szqe</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>How do I improve my gel application?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8szqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1l8orvk</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Something’s off and I don’t know what it is.</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8orvk</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1l8ppux</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>my gel x nails are in pain :(</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8ppux/my_gel_x_nails_are_in_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1l8qepm</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>I feel so sad 😭</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8qepm</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1l8t9mh</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Please help me.</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8t9mh/please_help_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1l8uvpg</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Gel X with summer colors + swirl design. These nails made me so happy</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rpne1qsgbb6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1l8om52</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>How do you prevent acrylic paint from ruining polish?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l8om52/how_do_you_prevent_acrylic_paint_from_ruining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1l8of64</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Why does my gel polish look like this?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8of64</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1l9gnp2</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>So far my favourite!!!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxc5elqwbg6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1l9gif2</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Finally a clean mani ✨️</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9gif2</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1l9frx3</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Greens!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9frx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1l9ekmn</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Urban Forestry</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9ekmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1l9dbkc</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Rainbow static</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u7d0sl3haf6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1l9ck2z</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Gel-x Appointment Length</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9ck2z/gelx_appointment_length/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1l9bdzf</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Glowing Morpho - Chamaeleon Nails (May PPU)</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9bdzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1l9b456</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Can’t stop staring ✨</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fzf0cs5epe6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1l9a8ss</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>dupe(s) of access denied by mooncat?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9a8ss/dupes_of_access_denied_by_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1l99rob</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Lilac and glitter</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l99rob</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1l99iks</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Alice is SO stunning ✨ perhaps my new favorite magnetic!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l99iks</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1l99dbu</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Need help with ombré for wife’s nails</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp57x5v1ae6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1l98r3x</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Paint It Pretty Polish</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l98r3x/paint_it_pretty_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1l98kxy</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Some nail stamping fun</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zwic8e33e6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1l9877h</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>my favorite nails so far</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q25xvshxzd6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1l9743g</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Shiftiest Mooncats 🦄🦄🦄</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8yqdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1l972le</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>And I said I didn’t like toppers 😅</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l972le</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1l96sir</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Ombrè Stars for Pride!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l96sir</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1l96jx3</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Just messing around on hold!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l96jx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1l96i0o</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Londontown "innovative" gel top coat.</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l96i0o/londontown_innovative_gel_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1l968si</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Some lil flowers</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l968si</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1l95ucr</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Iridescent topper recommendations?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wju4ccsm2b6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1l95qkl</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Rest in Peach with Celestine topper</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wlkkt68gd6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1l950kz</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Cotton Candy Swatches?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l950kz/fancy_gloss_cotton_candy_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1l94exm</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Color Match for Fenway Greens?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l94exm</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1l93y5n</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Ethereal Coffee Storm Apr25 PPU</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l93y5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1l93qzf</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Pride Puppy Presents Another Rainbow Mani ft. Atomic's Pastel Neons + Ball Drop</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l93qzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1l93cw8</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>My take on a sunset chrome with regular polish</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l93cw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1l9134p</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Went to the drugstore for a summer blue!</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krsuax5sic6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1l90yon</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat Winds of Fate?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a93c400yhc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1l90vl8</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Waiting on my nails to grow out after some over-filing happened but still wanted to practice so started making press on sets! (:</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zs91612chc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1l8yex8</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Favorite/Go-To Nail Polish Brands?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8yex8/favoritegoto_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1l8zp9f</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Polishes that match this blurple African Violet</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56dk4h379c6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1l8t9mq</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>swatched my entire collection</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8t9mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1l8zi3j</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>ILNP sugar plum</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7u15c00q7c6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1l8zc0b</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Polyvinyl Butyral Sensitivity and Peel-Off Base Coat Effectiveness</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8zc0b/polyvinyl_butyral_sensitivity_and_peeloff_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1l8z63n</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Can Seche Restore help streaking?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y04torkg5c6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1l8ykcd</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>May the Tickets Tempt You</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8ykcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1l8xgon</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Fandom Flakies Box</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8xgon/fandom_flakies_box/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1l8xa0x</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>What do I do😫</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouebqykcsb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1l8x9vq</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>ILNP - Flower Child</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8x9vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1l8x0a5</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>So obsessed with this shade!!!</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8x0a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1l8wx58</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>For the price of one Mooncat…</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a666rqospb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1l8wuyu</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨MARC JACOBS</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c87ovadpb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1l8wq68</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>First time doing a lazy gradient. Happy Pride y'all! 🌈</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8wq68</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1l8wpff</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>My Lover Dreams if the Sea in motion🌊</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nripad1aob6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1l8wc8m</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Rec request - a good Green that flashes bright warm colors (pink, red, orange, yellow) - chameleon, iridescent snake vibes</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8wc8m/rec_request_a_good_green_that_flashes_bright_warm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1l8vzat</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>My Lover Dreams of the Sea🌊🪸🪼</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8vzat</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1l8vnou</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Going to a punk/rock/metal festival, what a good excuse for fancy nails 🤘💚🖤</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8vnou</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1l8va6t</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Happy Pride ft. Gay Rainbow Frogs</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8va6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1l8v9tc</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>anyone else get annoyed of long nails and have to give them a chop once and a while?🩶</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8v9tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1l8v0ab</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Are these mannequin hands?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8v0ab</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1l8uuuh</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Trying out one of my new indies!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stutqh5abb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1l8ukr8</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Best Matte Top Coat?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8ukr8/best_matte_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1l8u44o</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Sheer polishes</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8u44o</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1l8u3je</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>55% tariffs ya, all!!!! Our polish is about to get so expensive!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txufpqg9ha6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1l8tuo1</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Deep Space velvet/cat-eye hybrid done with 3 bar magnets</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8vhbs3v14b6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1l8tjo3</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Breakfast at Moniques</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8tjo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1l8tgtz</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>traveling w polish</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8tgtz/traveling_w_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1l8t5bo</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>whats this polish?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/41zd2rloya6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1l8t2n9</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Bi/Pan flags for pride!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8t2n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1l8su8f</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>178 polishes in cart narrowed down to 9... Another Rainbow Connection Haul! (incl an EDM Mystery Bag)</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmn80idoua6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1l8styc</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Dupes for Shake your Shamrock</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8styc/dupes_for_shake_your_shamrock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1l8sng6</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Spacey polishes</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1d56f41xua6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1l8saml</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>This might be the most reactive magnetic I've tried</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln203cp5sa6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1l8rnq4</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>This polish photographs so pretty but</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5901d4uxma6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1l8rfpv</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Trans pride 🌈 and a reminder of why I hate creme formulas</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34inm9g3la6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1l8q7yy</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Getting gel polish has led to reigniting my love for nail polish</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzw4wstjz96f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1l8pgvd</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>ISO: Sheer, Iridescent Polishes That Mimic Feldspar Stones (Labradorite, Moonstone, etc.)</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9hkkqgg2a6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1l8n6cs</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Cuticula-Welcome to AZ Collection</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l8n6cs/cuticulawelcome_to_az_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1l9gqbs</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Where to buy cool gems &amp; stones for nail art</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l9gqbs/where_to_buy_cool_gems_stones_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1l9ez9v</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>My go-to design when my nails are short (the stars and moons glow in the dark)</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gwh0zm4sf6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1l9efp6</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>How many of you know Korean nail products?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l9efp6/how_many_of_you_know_korean_nail_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1l9bl5r</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>I painted Doodlebob nails</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9bl5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1l9b8gy</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>first tome trying hearts ❤️</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9b8gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1l9auvv</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Anaglyph Nail Art</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9auvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1l99956</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Sapphire ✨</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l99956</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1l96vod</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Ombrè Stars for Pride!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l96vod</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1l95e51</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>What should the thumb be??</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwkcvygqdd6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1l92c8b</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Inspired by princess peach 👑</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l92c8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1l91hzb</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Which are the best brands for jelly gel?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l91hzb/which_are_the_best_brands_for_jelly_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1l904by</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Red Chrome ❤️</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t47folv0cc6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1l8z6mf</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Happy pride! 🌈</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99fog46k5c6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1l8yx6n</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>My tech tried 3D work for the first time, juicy lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8yx6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1l8yhum</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Freestyle press ons I made for myself👩🏾‍🎤</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kl6biblt0c6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1l8xpb5</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>My cute set of nails 😋</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8xpb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1l8w15a</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Great Wave</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7m2s9j1ljb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1l8vgqn</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>In a different shape ✨</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx5xjkljfb6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1l8vcvs</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Something fun 🏁🎨</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8vcvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1l8uljd</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>These lines good or not?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8mma7ff9b6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1l8s14q</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Press ons by me :)</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrypmzw3qa6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1l8oy0x</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Pretty accurate for Summer 🔥</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e17m06onw96f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jun 13 08:12:45 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_15.xlsx
+++ b/data/collected_data/2025_06_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C877"/>
+  <dimension ref="A1:C1084"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15342,6 +15342,3525 @@
         </is>
       </c>
     </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1laabvl</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Can i go back to  add some new details</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxsyjq3kin6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1la9ojf</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Too long before my next refill?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vm1zt4jan6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1la9qdk</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>GOT MY NAILSS DONNEE!!! THEYRE GEL!!!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2ah4sa5bn6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1la9q1o</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Current stiletto pattern obsession</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjpgtcg1bn6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1la9p87</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>i gave myself rings of fire trying to take off gel. Don’t do what i did!</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la9p87</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1la9ne1</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Is this design as goofy as I think it is?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la9ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1la9m4c</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>in love with my new set</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgm2lxtp9n6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1la93s0</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Am I cooked?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du02zmck3n6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1la8sxp</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>this is why i learned to do my own nails .. (none of these were done by me)</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la8sxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1la8ox7</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Pet jellyfish</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7og97gunym6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1la9c0k</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Cute and subtle little flowers 🥰</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1a6lkybe6n6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1la8nmg</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Nail break</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la8nmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1la8j13</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Practice nail art on myself</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la8j13</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1la63j8</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>help pls</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1la63j8/help_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1la81ta</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Pride nails!</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la81ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1la80v7</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Loving my new set for vacation</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbs84824rm6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1la7scu</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>this color combo 😍😍</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2ei745lom6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1la7mmu</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>my moms nails :) chrome with Swarovski crystals ✨💅</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc6xcz2smm6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1la7bzo</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>can’t stop looking at them! 🐮</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la7bzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1la70b7</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Old set and new set!</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la70b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1la6w9i</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Is this more snakeskin like? 🧐</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wnpy1sw2fm6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1la68cn</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Summer Vibes 🫶</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la68cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1la67v2</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>in love with my nails you prefer square or oval</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc2krbs88m6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1la5p6a</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Any suggestions for a nail colour ? Haven’t done a manicure in 3 years. I’m warm autumn skin tone</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dmhe5i93m6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1la5nfe</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>First attempt at French nails</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la5nfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1la5fdv</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>First gel manicure - in love</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfz7828p0m6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1l9xwta</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Tips for how to get nails back to being healthy?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ciw1ncsq9k6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1la2qdm</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Beach inspired nails</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la2qdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1la33rx</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>i loved these nails</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ril8zkedfl6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1la3jbh</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Beginner needs help</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1la3jbh/beginner_needs_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1la4m8f</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>How do I make them less yellow?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la4m8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1la47yn</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Graduation/prom Nails</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la47yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1la56ef</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Hungry, hungry caterpillar theme</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7gxdd0zcyl6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1la48su</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>I love doing this</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58hnumeppl6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1la454l</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Cat eye</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tl56a0erol6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1l9p596</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Can I put a nail over this?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9p596</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1la41vz</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Sticky Tab Press Ons ontop of Gel?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1la41vz/sticky_tab_press_ons_ontop_of_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1la405b</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>adventure time 🩷🩵</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la405b</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1la3pa3</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>My nail girl slaying as usual 😍</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7nedp2pkl6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1la3mft</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Cat eye + chrome together is my new fav combo</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0gujhx0kl6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1la3hq8</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Some recent sets of mine 😘</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la3hq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1l9zrv9</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Can contact dermatitis show up weeks after application?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9zrv9/can_contact_dermatitis_show_up_weeks_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1la2vvl</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Nails popping off!? Why?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1la2vvl/nails_popping_off_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1la2nyo</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Butterflies</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgsc3vggbl6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1la29a8</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Loving my new set 💚</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t94idzay7l6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1la26oa</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Can I use gel x on top of builder gel?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1la26oa/can_i_use_gel_x_on_top_of_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1la1vrd</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>PIC for attention they’re crap I know! Soft Gel Nails for small nail beds advice?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebsdbq8w4l6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1la1cvp</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Looking for Good Platinum Press-On Nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1la1cvp/looking_for_good_platinum_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1la18oz</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Tried builder gel and it's my hold grail now!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la18oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1la163t</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Got my nails done for a fairy market last weekend 😍</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ymat4e3wyk6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1la157l</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Tried something new</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la157l</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1la12w2</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>tried semi cured gel strips!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la12w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1la0vmo</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Best set i’ve made :)</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la0vmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1la0umi</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Because you will appreciate the glow in the dark :)</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la0umi</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1la0ukz</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>BROOOOO I THOUGHT I HAD DISCOVERED A COOL HACK.</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1la0ukz/brooooo_i_thought_i_had_discovered_a_cool_hack/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1la0ema</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Excuse my pudgey fingers but I’m proud of how this set turned out!</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la0ema</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1la0511</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Strawberry Press-on Nails</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la0511</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1la09uk</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Koi fishes:3 Design vs Completion :×</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la09uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1la05xt</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>My go to nail salon is only $35</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la05xt</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1la03t3</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Is anyone selling gel nail polish bundles by color season?</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1la03t3/is_anyone_selling_gel_nail_polish_bundles_by/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1l9zrlp</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>how to grow my nails?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9zrlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1l9zrka</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Horrible and AGGRESSIVE nail salon experience just now</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvd9g3ulnk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1l9zp38</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>New set to match my girl &lt;3</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9zp38</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1l9zmhq</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>New nails 💙 Diamond Eyes DnD</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34l6e4ihmk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1l9z8j2</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Fruity nails for a fruity lady</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3de4pfcmjk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1l9z5y3</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Got soot sprite nails with lesbian pride colored dots</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tiv70323jk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1l9y4q7</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>What I got vs what I got inspo from! Credit goes to @buffandtweeze on ig. 🌊 ⚓ ⛵</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9y4q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1l9yigs</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>First time ever for acrylic marble and I am in love!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwgh5od6ek6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1l9x46p</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Chrome powder and top coat</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9x46p/chrome_powder_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1l9x9h0</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Tutorial! Chrome powder on regular polish ✨</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c8rw4kq15k6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1l9xac5</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Nail breakage tips</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9xac5</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1l9wv19</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Wanting to do gel nails - need some advice</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9wv19/wanting_to_do_gel_nails_need_some_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1l9x017</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>What do we think of these? Cute or is something off?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9x017</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1l9wuo3</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>i feel like fingernails have an odd shape. is there anything i can do about it?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik5tdwa22k6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1l9wopq</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>I ❤️ my nails</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf6smngv0k6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1l9wjn8</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>can i put press ons on this nail?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxigjchuzj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1l9wfyj</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Need advice asap</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsiqmsk3zj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1l9wi6y</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Rings of fire - how to minimise 2 weeks before my wedding</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4ix6ygkzj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1l9wlyt</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>1950’s Atomic Nails ✨</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9wlyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1l9wejf</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Aprés sizing</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9wejf/aprés_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1l9w30y</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>How damaged are these?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1sfad7kwj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1l9wcnz</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Flower set 🌸</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cquyhy0ayj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1l9vzuj</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Is tenderness normal? First time ever doing my nails, I went with press ons!</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjn9rlexvj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1l9uz5h</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cy6r70hmoj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1l9uyos</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Advice on at home gel pedicures</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9uyos/advice_on_at_home_gel_pedicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1l9vnak</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Do You Think You Should Be Charged Extra for Using 2 Colors?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9vnak/do_you_think_you_should_be_charged_extra_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1l9vby2</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>ALMOND SHAPED RUSSIAN MANI WITH A WHITE ON WHITE FRENCH 🤍</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cupyww65rj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1l9vb14</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Bi Flag Nails! 🩷💜💙 Happy Pride Month 🥰</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9vb14</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1l9v5gb</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>My vay cay set!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9v5gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1l9uvpi</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>cute manicure</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5zjvclynj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1l9ugbl</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Just asking for an advice</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9ugbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1l9u98y</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Best affordable lamp for gel?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9u98y/best_affordable_lamp_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1l9u4sw</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Everybody sould be Pride of themselves🥰</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldu41nrvij6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1l9u4f0</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Would I look better with oval/round nails?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9u4f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1l9u28c</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>WOULD YA LUUK AT DISS!!! 👏🏽</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1itsagzdij6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1l9t7sb</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Press on nails: always losing one or two nails CONSISTENTLY</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9t7sb/press_on_nails_always_losing_one_or_two_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1l9tmn1</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>new nails (ignore frank)</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enfrssaefj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1l9tbwm</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>By the sea 🌊</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acutoneddj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1l9ta24</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Hard gel in a bottle?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l9ta24/hard_gel_in_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1l9sucw</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Nails by Sam at Nails Amour</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpr85wj0aj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1la7wq9</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Summer vibes🍓🍉</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la7wq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1la7uwa</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Bloody Vampire Nails 🩸 - first time posting on this sub!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la7uwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1la7uw6</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Is there a polish similar to the photo?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mmgl2zbpm6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1la7lu5</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Self-Care Stamping</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la7lu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1la7g1v</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>How is everyone able to try all these brands?!</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1la7g1v/how_is_everyone_able_to_try_all_these_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1la7elv</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Dupe for the Flakies in ILNP Pitter Patter and Starlight?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la7elv</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1la6ih8</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>ILNP Hypnosis vs. Flip Side</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2hzultobbm6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1la5vf0</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Does anyone else consider the amount of ounces/mLs of a polish before buying?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1la5vf0/does_anyone_else_consider_the_amount_of_ouncesmls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1la5q9h</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Cirque dream within a dream - u mag</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la5q9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1la5g8z</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Preferred "Easy" Nail Art</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyh12gux0m6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1la4yai</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Yall</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la4yai</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1la4y86</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Indies FTW</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/065b4sg8wl6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1la4rlj</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Dam - Don’t Pee In The Pool</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la4rlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1la4ne5</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>How do I make this mani less yellow?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la4ne5</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1la3us0</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Hate this color on me. How to salvage??</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la3us0</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1la3dz4</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Burnt Bridges 🤎📀</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjghpjqvhl6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1la3ldb</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Thin brittle nails</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la3ldb</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1la3ggw</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>♥️🧡💛💚💙💜🖤🤎🩵🩷🤍</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la3ggw</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1la3c7d</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>First time painting my nails, glad they’re at least passable. 😆</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la3c7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1la31xb</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>This is DOOM LOOP 💅</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la31xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1la2d3b</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>ILNP Warped</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ys37xku8l6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1la29it</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Holo shorties😭🌈</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad0kc4r08l6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1la2203</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>dont forget about the simple things</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrqa29wa6l6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1la1yqi</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Just when I finalized my basket 😢</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zv5d81k5l6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1la1asc</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>First time doing manicures with Dazzle Dry, fungus!? Help!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td242mf6zk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1la17g2</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Dupe request - a couple of Mooncat polishes</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la17g2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1la0yp1</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>First try at ombre. Also ISO of individual fake nails for flatter curve fingas when I break one (or three)</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la0yp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1la0ojb</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Beyond Icarus</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la0ojb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1la0oe1</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Beyond Icarus</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la0oe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1la0ldt</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Swamp Gloss - Poot Poot Spoop</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la0ldt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1la08rp</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>ILNP Caroline</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la08rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1la06qy</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>God I love multichromes</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l8yqdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1l9zz36</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Alien Invasion 👽 🛸</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9zwk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1l9zx1q</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Guyyyysss.. Thermals and Shorties</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9zx1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1l9zveq</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Red Jelly DV Polish, pretty but not quite what I was looking for</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9zveq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1l9tcrb</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Mooncat Superclusterfck dupe?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9tcrb/mooncat_superclusterfck_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1l9tgu8</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>So I got both 712 (Ruth) and 563 (DND Red) from DND to compare.  See more details in post.</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9tgu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1l9uuno</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Does anyone recommend clean up products other than q-tips?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvzgr3urnj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1l9zmty</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>At this point, the monthly collabs are just Garden Path Lacquers distributors with extra steps for me.</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/762t719lmk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1l9zi9v</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Cat eye with regular polish</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hqyv68ullk6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1l9zhpt</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Holo Taco Ctrl Cutie</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9zhpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1l9zakk</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Flying Nimbus ✨☁️🩵☁️✨</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9zakk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1l9yz37</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Carved ILNP ☺️🧡</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9jtiy1ohk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1l9yuyy</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Smooth Moves Shrinkage?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qnc31htgk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1l9xlnn</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>LeChat Tressie</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9xlnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1l9xfru</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9xfru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1l9wkjk</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>New mom unexpected match</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k9j83510k6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1l9wgch</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>DIY Holo QDTC?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9wgch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1l9wg16</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Worth the hype- Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9wg16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1l9w7yb</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Before the Last Petal Falls</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9w7yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1l9w7m4</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>birthday mani! 🥳</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9w7m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1l9w1a4</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>The Favorite Cousin Discount</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9w1a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1l9v5a6</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>What nail shape would suit me?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9v5a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1l9uxly</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Casualties of moving and spilled acetone</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9uxly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1l9uat0</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Sheer Sparkly Shorties!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sc7n4vyvjj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1l9tegu</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>My new favorite yellow: Best-Teas by Rogue Lacquer!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9tegu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1l9t7n2</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Turquoise and more turquoise</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zwjsv5kcj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1l9t10d</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Wearing orange for my partner's graduation!</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1v0mf0d9bj6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1l9swk0</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Are base coats good forever?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9swk0/are_base_coats_good_forever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1l9sna8</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Cirques magnetics</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5nj9nfvk8j6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1l9s85w</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Sorry for the bad quality, I’m not a photoshop master, but do you think a tech would be able to do this? Also, thoughts? I want a mixture of Moroccan riad + baroque…. If that makes sense</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e46pouo5j6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1l9s607</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Stunning shift, I feel like a mermaid!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hjyxyp0a5j6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1l9s0l2</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>My regular polish mani at 20 days, a new record!!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9s0l2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1l9nfp8</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>I might've discovered a new magnetization style? What do we think? (Method in comments)</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l4lgerm67i6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1l9ruk3</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>OPI polish tacky</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9ruk3/opi_polish_tacky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1l9rqyh</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Glowing Wild</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9rqyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1l9quv9</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Anyone Else Do 2 Different Colors?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dahngvv8wi6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1l9qgpi</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>KBS Flash Forward vs. HT Playing with Sapphire</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9qgpi/kbs_flash_forward_vs_ht_playing_with_sapphire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1l9qfjx</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Cracks after applying dip</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9qfjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1l9py7c</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>How can a single polish be approximately 937,826 different colors?! Psilocybin by Clionadh is blowing my mind🤯🍄</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9py7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1l9pqun</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Sisters, Not Twins</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pnfnjsoaoi6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1l9okfc</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9okfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1l9odm3</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Pride Nails ~</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9odm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1l9n5hl</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Me trying to take a photo of my mani… my toddler: “HIGH FIVE!” 🖐️</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t6agb8yf5i6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1l9mxyx</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Chop Chop! Rockin' shorties :) - Severe nail damage warning</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9mxyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1l9mqan</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Went to a concert and didn't realize I would glow!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9mqan</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1l9mhty</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈🖤🩶Asexual "Ace" Pride Flag🤍💜🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9mhty</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1l9m2ou</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Where to buy Moth and moon nail polish (former shlee polish) in Europe?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9m2ou/where_to_buy_moth_and_moon_nail_polish_former/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1l9m2dq</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>La lluvia by cupcake polish</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xnzlb3yewh6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1l9lyfa</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Professional Cuticula Trimmer</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3cswlqgwvh6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1l9lvvr</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>A perfect glitter for a summer pool day!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9lvvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1l9kwlz</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Are there polish options that do not damage (or that strengthen) nails?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9kwlz/are_there_polish_options_that_do_not_damage_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1l9kda8</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>My 94 year old Lacquerista ♡</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9kda8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1l9ka05</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>could the new polished for days UFO Glow a possible dupe for Atomic’s Sour Apple Rings?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9ka05</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1l9k6mb</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Tips for polish longevity with water exposure?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9k6mb/tips_for_polish_longevity_with_water_exposure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1l9jd7w</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Can I use Seche Vite over DRK Magic Effect for Magnetics?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9jd7w/can_i_use_seche_vite_over_drk_magic_effect_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1l9j725</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>"Matte" glitters/metallics like these?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9j725</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1l9iu7w</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Don't sleep on LA Colors!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9iu7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1l9h017</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Waiting for someone to drop a collection in these colours</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l96b50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1l9gzgn</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Health anxiety after manicure</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l9gzgn/health_anxiety_after_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1la8mri</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Swag Nailz</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1843o67zxm6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1la8lvb</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Evangelion Nails</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b97toxoxm6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1la8l7z</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Nails I Did Today</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la8l7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1la88bf</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>@isabellanails amoo my talent</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la88bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1la4j1u</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>some press on nail sets I made :)</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la4j1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1la1ihn</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Some sets throughout the year</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la1ihn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1la0d87</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Shrek froggie balloon</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1isgkjbfsk6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1la03b0</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Pride Month</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la03b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1l9xv1y</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Dragon eye nail art 🐲</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpxnafpd9k6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1l9wv2h</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Summer Bees</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9wv2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1l9woix</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>press-ons</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9woix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1l9wjgd</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Gel polish for appliques?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l9wjgd/gel_polish_for_appliques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1l9v2ky</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Rainbow Jelly Fruit Salad Nails!!</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9v2ky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1l9rdg2</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Grab your friends, wear your florals!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9rdg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1l9q7qn</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Made them yesterday ^_^</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9q7qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1l9ljnn</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>My fairy core Queen press on nails... Soon to be joined by King 👑 Scroll through to see the individual nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9ljnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1l9iqxm</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>I love these</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l9iqxm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun 14 08:10:57 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_15.xlsx
+++ b/data/collected_data/2025_06_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1084"/>
+  <dimension ref="A1:C1273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18861,6 +18861,3219 @@
         </is>
       </c>
     </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1lb2yay</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>I’m usually a neutral girl</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb2yay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1lb2t1i</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Butter yellow 🧈</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4x6s41wgu6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1lb2sr5</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Do you tip your Russian Manicure Independent Tech?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lb2sr5/do_you_tip_your_russian_manicure_independent_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1lb2sop</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Summer cuties💕</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if3g5dgrgu6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1lb2ryh</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Best summer red for cool toned fair/medium skin?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lb2ryh/best_summer_red_for_cool_toned_fairmedium_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1lb264t</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Dremel on cuticles</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lb264t/dremel_on_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1lb1yiy</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>New month new nails</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bww6qabx6u6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1lb0985</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Could I have some advice on what to ask for to achieve the look I’d like from my nail tech?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb0985</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1lb0vnq</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Here are the other 9. Tho I went blind afterwards… but…oh well.</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb0vnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1lb1k79</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>My new set</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzxvxe4d2u6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1lb0yeg</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Fruit set!!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb0yeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1lb0dpe</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Summer season nail</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/th41tbj4pt6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1lazqdq</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>HELP finding gel closest to this polish</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lazqdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1lazpzb</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Summer gel mani @ home</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lazpzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1laz5sc</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Y’all help!!!!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laz5sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1laz4yr</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laz4yr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1laz49z</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Not perfect but my DIY Bi Pride nails</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxd812zrct6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1laz0u8</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Blueeee 😍😍🩵🩵</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjyqexytbt6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1layuu3</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>I'm not sure about this color with my skin tone.</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrhwsnme9t6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1laxts3</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Chrome over Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/spr9ypy70t6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1lay1kp</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>My first time making press ons how do i improve from here</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bh6mru5b2t6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1lay8t2</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Isolated chrome makes my brain confused</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lay8t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1lay6hd</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Super curved index nail</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lay6hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1laxoz6</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>look at nail.. nail done</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laxoz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1laxd10</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Tried layering some cat eye polishes</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k4pcoplpvs6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1lax1nl</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Gel X nails not flushed to nails</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lax1nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1lawbn6</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Well, my wife said I have good nails and should post it here, is it true?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lawbn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1law7mi</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1law7mi/gel_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1lavyys</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Can you soak off dip instead of drilling it off?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lavyys/can_you_soak_off_dip_instead_of_drilling_it_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1lavd3a</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>started doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejh440w3ds6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1lauqmb</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>The sunlight is hitting my new manicure so beautifully</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mnpyark7s6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1lauot2</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Very first personal set</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lauot2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1laukh4</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Summer Fun💕</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laukh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1laueir</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>My pride nails!</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acvkiswu4s6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1lau7wv</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>I made aquarium nails!🪸🪼✨</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lau7wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1lau6er</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Design vs Completion ~ Lavender sky 💜</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lau6er</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1lau4rk</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Guess how much I paid!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/da2pxxwj2s6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1lau21c</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>the last 2 sets I got, I’m getting my nails done tomorrow and I’m so excited! :D haven’t gotten acrylics in over a month</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lau21c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1lasmvz</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Washing Dishes</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lasmvz/washing_dishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1latsap</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Simple but beautiful</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd3jq1mlzr6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1latdee</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Opinions needed, how to further treat this</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1latdee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1lasrjp</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>I got my nails don’t today…I think she did it wrong…it’s supposed to color change but she should’ve put another color underneath. I feel like crying. It was pretty before it dried. I have social anxiety so now I have to go again to the place and I can’t stand it. How bad is it?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hker8e4brr6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1lasq0g</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Help with nail glue</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lasq0g/help_with_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1lap83h</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Gel X &amp; Luminary Saved My Nails</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lap83h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1l9zvgo</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>TAP manicure separat</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccdmxmvhok6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1la57y1</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>whats wrong with my nail?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la57y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1lan6ni</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Is this a bruise or an infection? Just found after removing press ons 😭</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nchb33o7kq6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1lanntq</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>How do I genuinely get press on nails to stay on for more than a few days</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lanntq/how_do_i_genuinely_get_press_on_nails_to_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1lao9jk</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>why is the white part of my nail clear?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lao9jk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1larvfq</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>I asked for ombre color</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ggqqr0fkr6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1lasewl</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>How'd I Do?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aoo3iirlor6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1larse3</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Lava lamp 💕✨</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1larse3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1larnyd</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Birthday/Vacation Nails</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1larnyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1lark99</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Is the gap too big - I just got them done at nail salon. I have bad anxiety but she said that she couldn’t put it any closer to the nail.</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lark99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1lark6c</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Tell my nail tech she ate..AGAIN😝🤭</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lark6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1larjeo</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Slime time, baby!</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1larjeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1laqwo9</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Nails turning upward?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ow3e66l5dr6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1laqkex</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>3 hours on my short anxiety bitten nails. Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laqkex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1laqbxn</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Strawberry nails 🍓</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvzkorep8r6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1laq1rz</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>🧈 for summer</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laq1rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1laptw3</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Summer nails!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fen3ouiy4r6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1laophi</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>This is Mickey, he loves nails</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5w28idwawq6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1lanx0k</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Confused about two contradicting methods from nail artists I went to</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lanx0k/confused_about_two_contradicting_methods_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1lanzha</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>got nail extensions for the first time!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lanzha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1lanxce</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Candyland set 🍭</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lanxce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1lanm6a</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Letting my butchered nails recover</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxy2kdxkoq6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1laninn</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Summer nails 🥵</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laninn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1lanefn</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Galaxy Nails</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3anspj0nq6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1lan87o</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>i love my nails 🩶!!!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lan87o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1lamsgv</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Green with rhinestones</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j22rnobniq6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1lamixv</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12qfm4etgq6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1lalvdk</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>pink, green, and gold 🩷</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtxm4236cq6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1lalsmc</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Yellow is so beautiful in the summer</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mpz7ss9mbq6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1lahjj3</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Hard as Hoof made me very itchy</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lahjj3/hard_as_hoof_made_me_very_itchy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1lahbli</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>This might sound dumb but I am so happy with my nail progress! (3 photos, goes from before to after)</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lahbli</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1lahsnu</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Part of toenail fell off and need help</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lahsnu/part_of_toenail_fell_off_and_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1lag52v</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Una Gella Nail Glue?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4hj6fdr6p6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1lac43y</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>New to acrylics.. question</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lac43y/new_to_acrylics_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1laij53</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Before and after 🥰</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laij53</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1laj9z8</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>These nails didn’t paint themselves... but they should be famous. haha</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/anzwh8mntp6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1lajnqj</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>broken nail - can I re-paint it?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v83i6jlfwp6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1lalbkm</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Almonds for the 1st time🌸</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txz4xf7a8q6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1lakw96</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Nail ideas</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lakw96/nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1lag5yd</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Is there any way to fix this on my own?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lag5yd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1laedja</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Bali holiday nails! Inspo by @claribelnailspy!</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laedja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ladus3</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Goth Robins egg inspired nails</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/foex3i0zmo6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1laczir</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Need some inspo!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laczir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1lakbrv</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Miami dusk</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lakbrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1lajgja</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Got a "dazzle dry" manicure YESTERDAY. It's completely ruined?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lajgja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1lajfh6</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>i need help finding the perfect denim blue color for my nails!!!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lajfh6/i_need_help_finding_the_perfect_denim_blue_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1laittk</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>My last two manis 💕</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laittk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1lait94</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>It's cute, right?!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pri9p228qp6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1laipjl</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>In my vampire era</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laipjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1laii4h</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Any fans of keeping it simple?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f24w0n2op6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1laia4t</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>First time getting acrylics 💅</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laia4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1lahysv</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>First time using builder gel</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lahysv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1lahm0t</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Which Base and Top Coat for Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lahm0t/which_base_and_top_coat_for_chrome_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1lahj2t</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Turned reg polish into gel</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lahj2t/turned_reg_polish_into_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1lah2cz</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Fresh fill 🌺</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lah2cz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1lags2k</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Starting to practice cartoons. What do you think of these Care Bears?🐻✨💕</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lags2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1lb3e1x</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Removing gel top coat off of press-ons?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lb3e1x/removing_gel_top_coat_off_of_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1lb34ob</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Nudes &amp; pinks recommendations (OPI)</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flyuchtrku6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1lb1uco</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>How strong is the magnetic pigment in Alice by ILNP?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lb1uco/how_strong_is_the_magnetic_pigment_in_alice_by/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1lb1c6b</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Is it still Brat summer?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb1c6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1lb1arl</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Faith</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2c63tsgzt6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1lb0lwf</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Was feeling lazy so I just want with press ons</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/250zgz6vrt6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1lb0ip2</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>First time using green polish</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb0ip2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1layj4s</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>What would you do?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1layj4s/what_would_you_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1laxgva</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Took three attempts because I kept bumping my nails before they were dry.</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkqiym4sws6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1laxb49</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>First post please be kind</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1laxb49/first_post_please_be_kind/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1lawiq3</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>I searched the sub w/o success. Does anyone know of a dupe for Manicurist Old Rose?</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lawiq3/i_searched_the_sub_wo_success_does_anyone_know_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1lawcve</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>LA Colors in all its glory</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lawcve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1lavzx1</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>May HHC Haul</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lavzx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1lavpj2</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Summer Blooming Hibiscus</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lavpj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1lav7y1</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Crackling Fire</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e6md8jhxbs6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1laubeu</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>pride nails 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laubeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1laubav</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Show off your emptiest bottle!</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6l5avz34s6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1latqyx</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>First time doing a gradient!</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uy5szdmbzr6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1lathbm</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>essie gel setter kinda sucks??</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lathbm/essie_gel_setter_kinda_sucks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1latga3</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Does anyone have Bloom Service by Dam Polish?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1latga3/does_anyone_have_bloom_service_by_dam_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1lat3qx</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Still fashionable with a broken arm take 2 😅 with an old thermal</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fqp3zp1ur6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1lasrmj</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Take 2: LynB As If vs. Alchemy Calveritas</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k708hdpbrr6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1lasnue</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Generally don’t wear warmer colors, but…</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lasnue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1laskyl</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>breast cancer / celebration of life nails</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laskyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1larvlh</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>🧟‍♀️ claws</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1larvlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1laruw8</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Bowling takes another victim</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laruw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1larmfx</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Got a cat eye manicure and I'm obsessed with it ✨</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/TWmNOLF.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1laqdjq</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Flower Nail Art</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onls7fy29r6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1larg21</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Need help finding a nail polish!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hoqrqdrp9r6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1larf4s</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>this nail polish is like MAGIC ✨</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4e606rbvgr6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1laqzos</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>💚 Glisten &amp; Glow Fab-Boo-Lous 💛</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8rafxmsdr6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1laqp6u</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Kaleidoscope of Butterflies🦋💙</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laqp6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1lapn64</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>What are the ingredients in the DRK magic effect top coat?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lapn64/what_are_the_ingredients_in_the_drk_magic_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1lapl3b</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>A bit of an ugly combo..</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2nj52x853r6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1lapbtg</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>LynBDesigns - Make A Splash</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bl1h53991r6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1lap3wk</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>1st Summer Neon</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hz54xmmzq6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1lap3se</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Lament</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lap3se</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1laoh55</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>First self-done set that got me unprompted compliments</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yai9y4exuq6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1laofmu</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>More Rogue love- my nails are GLOWING</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laofmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1laocgk</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Bloody themed nails</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laocgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1lanq7a</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Chicago Fire</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lanq7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1lamic5</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Mooncat - A Doll's House</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lamic5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1lamfwo</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Don’t you know that you’re toxic??</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lamfwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1lam70t</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Tried the new magnet technique to pretty cool results!</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1k1r3pqfeq6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1lam33s</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>My first skittle! All pinks 🩷</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06km4ciodq6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1lalytd</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Eleanor Doesn’t Want To Talk To You</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lalytd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1lalpn4</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>My nails so sparkly</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kaqssbiwaq6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1lalnmt</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Ethereal Beware Dupe</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lalnmt/ethereal_beware_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1laljuv</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>My polish matches my umbrella!</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laljuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1lali7k</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Your favourite magnetic polishes please!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lali7k/your_favourite_magnetic_polishes_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1lalc6q</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Funny Business Lacquers is open!</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lalc6q/funny_business_lacquers_is_open/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1lakpbk</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Dupe request! Baroness X Matcha. Trying to skip HHC this month</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1j8mgyj3q6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1lakmu8</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Strength of Courage</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lakmu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1laklcv</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Hypnosis is definitely Hypnotizing</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/RGZerEb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1lajqfl</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Camera breaking pink</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lajqfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1lajgr5</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Can I use a quick drying top coat over this one? My nails got messed up in my sleep. 🥲</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vobktpu1vp6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1laie0x</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Happy Friday the 13th! Apocalypse Polish is having a 13% off sale</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kd9m0bvymp6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1lahk9k</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>ILNP Poison 🍎</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lahk9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1lahfz2</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>I did it! I finally nailed the velvet effect without the horseshoe magnet! Cannot keep my eyes off of my nails!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ycqjkbh9gp6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1lagrvb</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>A-england is closing?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofrpw0olbp6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1lagk2w</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>this combo 🧡🍊🍑</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lagk2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1laggbe</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈💚🤍Abrosexual Pride Flag🤍🩷🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laggbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1lagbbx</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Cock a doodle doom + flower child</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lagbbx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1lafytr</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>First time trying Holo Taco Blue Rizzler</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lafytr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1laem64</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I rarely wear such a bold purple... Have to admit I'm not sure how I feel about this one!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laem64</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1la7ldg</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>First ILNP ever 🔥</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/agbvh3fgmm6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1ladfrz</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Recent manis🪻</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ladfrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1labuml</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Not vibing with this weeks colour but my application was neat soooo 🙆🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr4tclij1o6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1labe0r</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Trying to find my best “my nails but better” combo</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1labe0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1lab6sb</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Silver/purple magnetic?</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lab6sb/silverpurple_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1lb3gjb</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6x5qhsoou6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1lay3ij</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Japan themed nails 🍡🎋</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lay3ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1laxtba</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Fishing nails for father's day</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkah3ue30t6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1lawp6n</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Bows</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lawp6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1law9x2</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Cleopatra 💅🏼 💫</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1law9x2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1lauwrs</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>My first set of DIY press on nails</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zdhigc89s6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1laulux</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laulux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1lau93j</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>I made aquarium nails!🪸🦀✨</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lau93j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1lastye</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>My Sailor Moon Press Ons ✨️💅🏼</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dix7fb3urr6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1lakcg3</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Miami dusk</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lakcg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1lak1in</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>did my doggies as nail hippers</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lak1in</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1lajqam</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Summer rainbows 🌈  @sueznails @phillynails</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1crfquvxwp6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1laizh0</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Art Inspired Set with the inspo</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1laizh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1lai3da</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>🍄 mushy season</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pp6h0q8lp6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1lagqxh</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Starting to practice cartoons 🖌️🎨What do you think of these Care Bears?🧸💕✨</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lagqxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1lagnv5</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Foils..!</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lagnv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1lagb52</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Trying out this design for Pride month 💜</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lagb52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1labrd2</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Design for me 🍓🍉💋❤️</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kx2hd2f0o6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1laaone</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Gold glitter on black 🖤</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a09klnqymn6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun 15 08:10:49 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_15.xlsx
+++ b/data/collected_data/2025_06_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1273"/>
+  <dimension ref="A1:C1469"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22074,6 +22074,3338 @@
         </is>
       </c>
     </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1lbuq3y</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Any other guys get their toes done? What’s your take ladies?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzk0x6tzo17f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1lbuduq</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>I’m a guy and I’m scared (and kinda clueless)</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbuduq/im_a_guy_and_im_scared_and_kinda_clueless/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1lbuaq8</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Summerween 🍓🕷️</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/do2f8mewj17f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1lbtqdl</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>A bit of a throwback but I made a Judy charm!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbtqdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1lbtnzs</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Happy Pride.</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbtnzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1lbtld3</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>THIS IS SUCH A CUTE BABY BLUE COLOR!!!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbtld3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1lbtaql</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Sizing in gelx nail kits</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbtaql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1lbsnpp</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Would you ask for a redo?</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5olrnwkp017f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1lbsc1h</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>I said surprise me and couldn't have left happier!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhpcogr6x07f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1lbs5l2</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>cake nails :)</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/36n19q46v07f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1lbrxuc</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Silver Cat-Eye and Chrome Stars</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/btvoyq8ts07f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1lbrv3f</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>It's cute. right?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkt9i0cvr07f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1lbrgpz</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Do my nails look nice? I paid like $70 with tax</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbrgpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1lbr1wr</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Nails for my sister</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbr1wr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1lbqxt8</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>🌊Ocean theme gel mani</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbqxt8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1lbqftn</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Are these good?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aboo23phd07f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1lbqby7</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>soft chaos in polish form, bc why not</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbqby7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1lbqbn9</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Blue gelx cateye</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbqbn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1lbpvcb</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Gelx ok in extended periods of water?</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/681olb4x707f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1lbpnxb</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Just a guy who has pretty feet</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7eirr9m507f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1lbpns7</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Got a beautiful red from Ulta the other day 🩷</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbpns7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1lbplgj</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Happy pride! 🌈</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk9tvnc9507f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1lbpdge</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Gold to match my dupatta ✨</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux4c84f3307f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1lbp8f6</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Some more Pride nails 🌈</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68p3arvq107f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1lbp80q</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>BIRTHDAY NAILS 💅</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wesxt9wm107f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1lbp6kj</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Nail day is best day</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bku8viw8107f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1lbp3iq</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>orange crush 🍊</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi3ylh2f007f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1lbow2u</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Nezuko nails ❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbow2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1lbouzb</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Pastel rainbows for pride month 🌈</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4ilfbf5yz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1lbou3o</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbou3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1lborsw</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>My new set, I love the color 🩷</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ct7rpygbxz6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1lbop9x</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>CROC SUMMER</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbop9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1lboh55</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Progress</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lboh55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1lbodtu</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Acrylics 💙</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcxmehwhtz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1lbod3e</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Acrylic set ❤️</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vytzsrsatz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1lboamm</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>💕Press ons 💕</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxgs2g6nsz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1lbo4lb</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>favourite nails of my actual life</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbo4lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1lbnt3u</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Fun vacation nails</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvy3kvgynz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1lbnszi</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Gel x as press ons?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbnszi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1lbng9g</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Liquid gel set issue</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbng9g/liquid_gel_set_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1lbnots</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Orange Chrome 🍊</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqgjxn5umz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1lbmwsg</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Going with something simple</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyglttoofz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1lbmw6k</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>I think red is the winning color</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qofr2refz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1lb609m</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Salon hygiene question</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lb609m/salon_hygiene_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1lbmouu</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Need advice on Price of nails with charms tech does not have</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbmouu/need_advice_on_price_of_nails_with_charms_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1lbmkzk</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>My recreation of an allycoolcat nails</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbmkzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1lbmioq</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>✨️First Time Trying Gel Strips✨️</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9amitg7cz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1lblnik</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Orange chrome for summer 🧡</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lblnik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1lbmfe0</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Thumb nail broke, do I just clip it off? Or is there a resin that can help?</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uoiez77ebz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1lbmezt</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>I'm confused... can I put the UV gel polish on top of 'acrylic' false nails? Or is the gel for natural nails.</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbmezt/im_confused_can_i_put_the_uv_gel_polish_on_top_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1lbm80h</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>What should I add?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2wmgadk9z6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1lbm4s9</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Blue tips w/cherry</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84z8nwfs8z6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1lbm200</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>scuffed new nails somehow, anyway to fix without going back to the salon?</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbm200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1lbm0mu</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ffa7fht7z6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1lblllr</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>ORLY Builder Gel?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lblllr/orly_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1lbk3c2</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>vaca nails I did on myself 💖</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbk3c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1lbhz01</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Why the discoloration?</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ts8149xhay6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1lbjsol</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Another fabulous mani, summer loving</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbjsol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1lbh124</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Can't tell if it's a gel allergy or my regular stress blisters</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbh124/cant_tell_if_its_a_gel_allergy_or_my_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1lbjo8v</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>pink nails to match my labubu 😁💖</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbjo8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1lbj5yl</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Another set 😍</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbj5yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1lbiu3i</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Pre Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pczs2ichy6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1lbiu37</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Best shape for my nails?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbiu37</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1lbityb</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Help me pls</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbityb/help_me_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1lbit1l</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7arshw3hy6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1lbirbw</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>First time doing gel extensions at home help!</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbirbw/first_time_doing_gel_extensions_at_home_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1lbiq47</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Summer vibes?</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4kqvfiggy6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1lbinru</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Do my nails look weird?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0ze9urxfy6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1lbi2zd</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>I loved them</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbi2zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1lbhvni</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>back to my natural nails and just gel polish</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6fyh94r9y6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1lbhtu2</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbhtu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1lbhtq2</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbhtq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1lbhq8e</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Which color should i paint my nails?</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na4zyp3j8y6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1lbhj03</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Tried to do my own rose quartz nails.</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbhj03</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1lbhdkz</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>My natural nails 💅 🌸</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcszhkmv5y6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1lbh8y4</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>I tried some blooming gel layering. I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbh8y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1lbh3dg</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>I’m new to Dip. Help!</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbh3dg/im_new_to_dip_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1lbgc3c</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>What I got vs What I asked for, inspired by design_de_unhas_lindass on IG</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbgc3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1lbgz6d</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Are my nails to short even for foodservice?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbgz6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1lbdo1z</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Can I do gel on these post-acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag9e2abbdx6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1lbfwoo</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>29/F, never been to a nail salon for job-related reasons but might go to prep for a friend’s wedding. Need advice.</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3pt9av5ux6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1lbg5wu</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Short nails again. Honestly, long ones are beautiful, but they just don’t let me live</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tam6co4wx6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1lbg04n</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>New to This!</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbg04n/new_to_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1lbfj9p</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>The perfect summer nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbfj9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1lbfasa</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Beautiful and Simple Press Ons</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rti5g78npx6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1lbf76m</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Pretty in pink 💕</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38d0oqt0px6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1lbf5gi</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>so in love with this pink white ombré set💖✨</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbf5gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1lbf1rz</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Can I add iridescent to my TAP  (builder gel/hybrid) nails?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbf1rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1lbey1e</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>i was going to do pride nails but the cat eye chrome combo caught my eye</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fiv0f802nx6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1lbee94</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Question about nail care</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59ulvegyix6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1lbe3mq</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Which shape for me? I gravitate toward a super pointy medium almond, but I'd appreciate others' input.</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbe3mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1lbdu8l</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Labradorite nail art</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbdu8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1lbdqh4</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>It’s time to get  f💥u🦠n🔸k👾y🦕</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbdqh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1lbdgdg</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnlwix6qbx6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1lbdegv</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Any press on nail lovers?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbdegv/any_press_on_nail_lovers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1lbdbrq</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Cat nails for cat lovers :3 🐈</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbdbrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1lbcwiv</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Prince inspired nails</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z19ulv8g7x6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1lbcsyb</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>HELP!!! Contact Dermatitis Questions</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lbcsyb/help_contact_dermatitis_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1lbcsxh</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>My attempt at gradient Pride nails 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbcsxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1lbcrre</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Cuticle machine?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99vhna6f6x6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1lbuxet</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>bi pride nails</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbuxet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1lbujwp</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Can anyone recommend cremes in this shade? Lmao</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcqp070ym17f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1lbsje1</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Weird Science</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mkugzm1ez07f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1lbs53o</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Can everyone share there favorite velvet/cat eye polishes?</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbs53o/can_everyone_share_there_favorite_velvetcat_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1lbrwn4</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Orly mystery blue</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbrwn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1lbrm6m</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>How similar are Dam Year of the Dragon vs Sassy Sauce Chicago Fire?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbrm6m/how_similar_are_dam_year_of_the_dragon_vs_sassy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1lbpb4l</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Summer Skittle</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvjl61xg207f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1lbr6u9</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>For a moment I thought I'd duped myself.</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbr6u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1lbr2qx</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Ready for summer! *Inspiration included*</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbr2qx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1lbqmxd</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>I present, the Indecision Skittle!</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbqmxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1lbq6n8</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Recommendation for a shimmer topper</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycyydvg0b07f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1lbpzmm</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Summer nails sorted!</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/keu9txv2907f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1lbpig3</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Cirque Mobius</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbpig3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1lbpdmx</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Gimme all your cheeriest brightest mani’ please!</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbpdmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1lbpcwf</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Rec request: Flakie and shimmer packed Teals/Turquoises/Greens to browse</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbpcwf/rec_request_flakie_and_shimmer_packed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1lbp7zv</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>pride manis 2 &amp; 3</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbp7zv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1lbp293</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Pride Mani</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b517ui94007f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1lbp13u</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Wearing Warped at Warped Tour</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxqsvxaszz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1lboh5v</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Mooncat Koi whiskers vs. Fancy Gloss Sundown vs. Holo Taco Rage bait. For Science!</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lboh5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1lbo5k8</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Half Year Mani Journal!</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bol3ab8arz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1lbo14h</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Wicked Sorcery</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d4tgm2a2qz6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1lbny93</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>My first Ethereal Lacquer - WOW!</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbny93</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1lbnmof</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>The good things</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bs8c796amz6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1lbndtk</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Colors R Poppin’</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbndtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1lbn0wu</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Call me Skipper! ⛵️</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbn0wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1lbm3cl</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>How to make my nail lines normal?</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9skdang8z6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1lblwgq</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Promo code for Polished for Days?</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lblwgq/promo_code_for_polished_for_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1lbllt1</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>First Fancy Gloss order. I am impressed</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbllt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1lble0v</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Dupe requests!</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q26leqli2z6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1lbld2e</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Happy (belated) Friday the 13th 🛶🩸🔪 🌊</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbld2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1lbkgrp</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Magnetic Magic!</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ulk8rqtluy6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1lbjqrb</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Lo-Fi Lavender ✨baby’s first Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbjqrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1lbjd3e</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Does poundage of horseshoe magnets make a difference?</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbjd3e/does_poundage_of_horseshoe_magnets_make_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1lbiznf</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>My version of pride nails</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wew7w47dhy6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1lbiqy2</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>1 coat of ILNP Warped looks so ethereal</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbiqy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1lbimvy</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Any suggestions/swatches for a purple sheer with green blue shimmer?</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbimvy/any_suggestionsswatches_for_a_purple_sheer_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1lbigqf</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Matchy Mismatch</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbigqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1lbi258</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>What’s your favorite purple?</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbi258/whats_your_favorite_purple/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1lbhjev</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Estate sale nail polish</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbhjev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1lbgxmk</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>First time doing my nails in over a year and it makes me so happy!</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/usovmypd2y6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1lbgw3i</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Summery two colors!</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbgw3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1lbgnm7</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Bordeaux</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmmecn770y6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1lbghkx</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Poems for a Harvest Moon 😍</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbghkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1lbg75n</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Boutique or Indie?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbg75n/boutique_or_indie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1lbg0bw</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>The many shades of Infinite Nebula (solar/thermal)☀️🌡️</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbg0bw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1lbflca</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Harley Noticeable</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbflca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1lbfdhi</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Help identifying this bottle?</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbesiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1lbezqo</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Circular Magnets</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbezqo/circular_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1lbdbuo</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>If you had to pick a single polish, what would you say your all-time favorite was?</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbdbuo/if_you_had_to_pick_a_single_polish_what_would_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1lbczxm</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Another Pride mani 🌈</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbczxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1lbdsg7</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Fitting lacquer for Hell 😿📝</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0qm60cwdx6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1lbdj0f</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Holy smokes Fancy Gloss is GOOD!!!</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbdj0f/holy_smokes_fancy_gloss_is_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1lbdgjd</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Is My Ass on Fire, Be Honest</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbdgjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1lbd5rz</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>For those with these swatch books</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyk4a8uf9x6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1lbczi6</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>For Liberty and Justice for all</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbczi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1lbcv39</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>*Physically* Mixing lacquer and gel?</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbcv39/physically_mixing_lacquer_and_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1lba69t</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Nail polish thinner alternatives?</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lba69t/nail_polish_thinner_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1lbc5o5</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Simple and elegant ✨</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbc5o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1lbc2zd</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>matching my nails to my groomsman suit &gt;&gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uic7nmn21x6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1lbbwio</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>What’s the spookiest polish you own?</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbbwio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1lbbu69</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Using quick dry drops over magnetic polish</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbbu69/using_quick_dry_drops_over_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1lbb4hw</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Trying to get more into blues</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lmle2hmtw6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1lbb00a</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Polishes for Days Haul and Swatch Comparisons</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbb00a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1lbaxet</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Holo for the beginning of June</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbaxet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1lbablz</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Are gels ever dangerous if I'm only painting acrylics with them?</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lbablz/are_gels_ever_dangerous_if_im_only_painting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1lb9o62</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Omggg love this one too!</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb9o62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1lb96ip</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈🩷💜Bisexuality Pride Flag💜💙🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb96ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1lb90i9</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>House of Hades has been dethroned</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/09z8fhilcw6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1lb8www</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Holy shift!!!</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb8www</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1lb8ihj</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Need ID on these 2 nail polish bottles</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26hui9l67w6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1lb8cv7</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>ILNP Bluebird</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb8cv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1lb81v1</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Anyone know of any brands that use short medium/ wide nail polish brushes?</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lb81v1/anyone_know_of_any_brands_that_use_short_medium/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1lb7fds</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>When the Polish Matches the Sleeve</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8tdte56yv6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1lb68p1</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>🥀 i love thermals</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9ugnnh2mv6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1lb4k00</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Egg yolk nails 🍳</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5a8eunnt1v6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1lb4d1u</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>WIDE BRUSH REPLACEMENT FOR ESSIE???</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lb4d1u/wide_brush_replacement_for_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1lbsc9c</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>did my own sapphic pride nails 🌈</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbsc9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1lbrdu3</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>I'm no professional at all, but I enjoy this nail polish combo.</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4hg8fdlm07f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1lbqzf2</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>❤️mickey mouse theme nails</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbqzf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1lbqysw</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>🌊Ocean themed gel mani</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbqysw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1lbp3k2</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>First go at making press on nails</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/344h5xjf007f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1lbocag</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>💕press ons💕</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbocag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1lblvtk</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Phoenix-Inspired Nail Art Set – Hand Painted</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/he3ov1oo6z6f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1lbk9yl</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>how to get it clean?</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abmhp5f1ty6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1lbjdyd</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Happy pride, again!</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbjdyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1lbjdaf</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Getting junky for June 🌈</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbjdaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1lbiwbl</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Loving this summer set</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfccu11thy6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1lbio5q</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>I had to hit y’all with another set 😝💕</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbio5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1lber2e</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Nail Art Inspired by Album Covers 💿</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lber2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1lbeeyq</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Neon colors all summer long :)</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbeeyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1lbbyso</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>first time doing gel-x on my friend!</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kg1ie0c50x6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1lbbdfc</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Investing to nail art brushes?</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lbbdfc/investing_to_nail_art_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1lb8zw0</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>@isabellanails nails of a bride</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uopxq9jhcw6f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1lb7pdy</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>My first attempt at watercolor nail art</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb7pdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1lb7l1m</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Custom Chrome press on set!🌌🪩</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb7l1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1lb4uxf</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>🩵🩵</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lb4uxf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>